<commit_message>
updates for December 2023 - also see a power point
</commit_message>
<xml_diff>
--- a/CHANGE/Interesting_Patterns.xlsx
+++ b/CHANGE/Interesting_Patterns.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t xml:space="preserve">landed_year</t>
   </si>
@@ -38,73 +38,70 @@
     <t xml:space="preserve">perc_change_lbs</t>
   </si>
   <si>
+    <t xml:space="preserve">MS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BAY SAINT LOUIS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRANDON</t>
+  </si>
+  <si>
     <t xml:space="preserve">LA</t>
   </si>
   <si>
-    <t xml:space="preserve">AMELIA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">APALACHICOLA</t>
+    <t xml:space="preserve">CHARENTON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DESTIN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GULF BREEZE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISLAMORADA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JACKSON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MILTON</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MYRTLE GROVE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PLACIDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POMONA PARK</t>
   </si>
   <si>
     <t xml:space="preserve">TX</t>
   </si>
   <si>
-    <t xml:space="preserve">ARANSAS PASS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BIG PINE KEY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EASTPOINT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ESTERO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FORT PIERCE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GIBSON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GREEN COVE SPRINGS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HIALEAH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HORSESHOE BEACH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HUDSON</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NAVARRE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PANACEA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PERRY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SANIBEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SOUTHPORT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SUWANNEE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WESTWEGO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YOUNGSTOWN</t>
+    <t xml:space="preserve">PORT MANSFIELD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEMINOLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPRING HILL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUGARTOWN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TAVERNIER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">YOUNGSVILLE</t>
   </si>
 </sst>
 </file>
@@ -464,7 +461,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2005</v>
+        <v>2015</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -473,24 +470,24 @@
         <v>9</v>
       </c>
       <c r="D2" t="n">
-        <v>24018</v>
+        <v>261975</v>
       </c>
       <c r="E2" t="n">
-        <v>5747</v>
+        <v>90096</v>
       </c>
       <c r="F2" t="n">
-        <v>7473</v>
+        <v>97921</v>
       </c>
       <c r="G2" t="n">
-        <v>-78.71</v>
+        <v>-71.23</v>
       </c>
       <c r="H2" t="n">
-        <v>10.96</v>
+        <v>320.82</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1989</v>
+        <v>2011</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -499,19 +496,19 @@
         <v>11</v>
       </c>
       <c r="D3" t="n">
-        <v>3297314</v>
+        <v>388</v>
       </c>
       <c r="E3" t="n">
-        <v>16303900</v>
+        <v>3104</v>
       </c>
       <c r="F3" t="n">
-        <v>30245750</v>
+        <v>3598</v>
       </c>
       <c r="G3" t="n">
-        <v>-58.21</v>
+        <v>-57.52</v>
       </c>
       <c r="H3" t="n">
-        <v>-5.64</v>
+        <v>142.5</v>
       </c>
     </row>
     <row r="4">
@@ -525,24 +522,24 @@
         <v>13</v>
       </c>
       <c r="D4" t="n">
-        <v>1841347</v>
+        <v>4565</v>
       </c>
       <c r="E4" t="n">
-        <v>2844155.5</v>
+        <v>521</v>
       </c>
       <c r="F4" t="n">
-        <v>3091188</v>
+        <v>566</v>
       </c>
       <c r="G4" t="n">
-        <v>-54.18</v>
+        <v>-66.09</v>
       </c>
       <c r="H4" t="n">
-        <v>0.86</v>
+        <v>196.43</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>2007</v>
+        <v>1986</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -551,24 +548,24 @@
         <v>14</v>
       </c>
       <c r="D5" t="n">
-        <v>602</v>
+        <v>10707</v>
       </c>
       <c r="E5" t="n">
-        <v>1197</v>
+        <v>7552</v>
       </c>
       <c r="F5" t="n">
-        <v>1471</v>
+        <v>15445</v>
       </c>
       <c r="G5" t="n">
-        <v>-52.49</v>
+        <v>-51.22</v>
       </c>
       <c r="H5" t="n">
-        <v>-10.01</v>
+        <v>140.34</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1995</v>
+        <v>1993</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
@@ -577,24 +574,24 @@
         <v>15</v>
       </c>
       <c r="D6" t="n">
-        <v>1115202</v>
+        <v>152279</v>
       </c>
       <c r="E6" t="n">
-        <v>4033485</v>
+        <v>192525</v>
       </c>
       <c r="F6" t="n">
-        <v>6389958</v>
+        <v>318049</v>
       </c>
       <c r="G6" t="n">
-        <v>-66.19</v>
+        <v>-75.12</v>
       </c>
       <c r="H6" t="n">
-        <v>5.76</v>
+        <v>446.8</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>2010</v>
+        <v>1979</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
@@ -603,102 +600,102 @@
         <v>16</v>
       </c>
       <c r="D7" t="n">
-        <v>1046</v>
+        <v>305953</v>
       </c>
       <c r="E7" t="n">
-        <v>1046</v>
+        <v>473696</v>
       </c>
       <c r="F7" t="n">
-        <v>1238</v>
+        <v>1391085</v>
       </c>
       <c r="G7" t="n">
-        <v>-59.92</v>
+        <v>-94.55</v>
       </c>
       <c r="H7" t="n">
-        <v>2.55</v>
+        <v>100.27</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>1993</v>
+        <v>2016</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
       </c>
       <c r="D8" t="n">
-        <v>586</v>
+        <v>1800</v>
       </c>
       <c r="E8" t="n">
-        <v>1197</v>
+        <v>1600</v>
       </c>
       <c r="F8" t="n">
-        <v>1978</v>
+        <v>1722</v>
       </c>
       <c r="G8" t="n">
-        <v>-61.43</v>
+        <v>-75.44</v>
       </c>
       <c r="H8" t="n">
-        <v>-9.01</v>
+        <v>74.76</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2005</v>
+        <v>1993</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
         <v>18</v>
       </c>
       <c r="D9" t="n">
-        <v>23266</v>
+        <v>182920</v>
       </c>
       <c r="E9" t="n">
-        <v>15673</v>
+        <v>833251</v>
       </c>
       <c r="F9" t="n">
-        <v>20381</v>
+        <v>1376521</v>
       </c>
       <c r="G9" t="n">
-        <v>-91.02</v>
+        <v>-64.89</v>
       </c>
       <c r="H9" t="n">
-        <v>8.9</v>
+        <v>52.01</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2009</v>
+        <v>2007</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C10" t="s">
         <v>19</v>
       </c>
       <c r="D10" t="n">
-        <v>2021</v>
+        <v>151</v>
       </c>
       <c r="E10" t="n">
-        <v>2021</v>
+        <v>152</v>
       </c>
       <c r="F10" t="n">
-        <v>2420</v>
+        <v>187</v>
       </c>
       <c r="G10" t="n">
-        <v>-68.9</v>
+        <v>-55.58</v>
       </c>
       <c r="H10" t="n">
-        <v>-9.13</v>
+        <v>308.11</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>1989</v>
+        <v>2020</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
@@ -707,24 +704,24 @@
         <v>20</v>
       </c>
       <c r="D11" t="n">
-        <v>98400</v>
+        <v>1038</v>
       </c>
       <c r="E11" t="n">
-        <v>90470</v>
+        <v>3440</v>
       </c>
       <c r="F11" t="n">
-        <v>167832</v>
+        <v>3440</v>
       </c>
       <c r="G11" t="n">
-        <v>-53.75</v>
+        <v>-50.55</v>
       </c>
       <c r="H11" t="n">
-        <v>-12.84</v>
+        <v>60.19</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>1987</v>
+        <v>2010</v>
       </c>
       <c r="B12" t="s">
         <v>10</v>
@@ -733,253 +730,175 @@
         <v>21</v>
       </c>
       <c r="D12" t="n">
-        <v>290955</v>
+        <v>7681</v>
       </c>
       <c r="E12" t="n">
-        <v>296</v>
+        <v>10369</v>
       </c>
       <c r="F12" t="n">
-        <v>591</v>
+        <v>12269</v>
       </c>
       <c r="G12" t="n">
-        <v>-99.63</v>
+        <v>-64.51</v>
       </c>
       <c r="H12" t="n">
-        <v>-8.05</v>
+        <v>232.08</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1991</v>
+        <v>2008</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D13" t="n">
-        <v>127331</v>
+        <v>2810</v>
       </c>
       <c r="E13" t="n">
-        <v>61231</v>
+        <v>2248</v>
       </c>
       <c r="F13" t="n">
-        <v>105910</v>
+        <v>2709</v>
       </c>
       <c r="G13" t="n">
-        <v>-63.38</v>
+        <v>-73.76</v>
       </c>
       <c r="H13" t="n">
-        <v>10.43</v>
+        <v>85.97</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>2008</v>
+        <v>2010</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D14" t="n">
-        <v>1501</v>
+        <v>4807</v>
       </c>
       <c r="E14" t="n">
-        <v>1501</v>
+        <v>4351</v>
       </c>
       <c r="F14" t="n">
-        <v>1809</v>
+        <v>5148</v>
       </c>
       <c r="G14" t="n">
-        <v>-76.58</v>
+        <v>-78.84</v>
       </c>
       <c r="H14" t="n">
-        <v>-14.28</v>
+        <v>141.44</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1985</v>
+        <v>2016</v>
       </c>
       <c r="B15" t="s">
         <v>10</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D15" t="n">
-        <v>4480</v>
+        <v>1073.5</v>
       </c>
       <c r="E15" t="n">
-        <v>4684</v>
+        <v>2161.03</v>
       </c>
       <c r="F15" t="n">
-        <v>9772</v>
+        <v>2325</v>
       </c>
       <c r="G15" t="n">
-        <v>-60.89</v>
+        <v>-51.72</v>
       </c>
       <c r="H15" t="n">
-        <v>-10.69</v>
+        <v>112.15</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>2001</v>
+        <v>2015</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D16" t="n">
-        <v>12848</v>
+        <v>2661</v>
       </c>
       <c r="E16" t="n">
-        <v>12091</v>
+        <v>705</v>
       </c>
       <c r="F16" t="n">
-        <v>17244</v>
+        <v>766</v>
       </c>
       <c r="G16" t="n">
-        <v>-68.06</v>
+        <v>-72.71</v>
       </c>
       <c r="H16" t="n">
-        <v>-9.43</v>
+        <v>151.99</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>2005</v>
+        <v>1987</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D17" t="n">
-        <v>1024</v>
+        <v>80053</v>
       </c>
       <c r="E17" t="n">
-        <v>1281</v>
+        <v>123</v>
       </c>
       <c r="F17" t="n">
-        <v>1666</v>
+        <v>246</v>
       </c>
       <c r="G17" t="n">
-        <v>-58.12</v>
+        <v>-88.9</v>
       </c>
       <c r="H17" t="n">
-        <v>-14.67</v>
+        <v>637.41</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1996</v>
+        <v>2000</v>
       </c>
       <c r="B18" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D18" t="n">
-        <v>202829</v>
+        <v>1096</v>
       </c>
       <c r="E18" t="n">
-        <v>198677</v>
+        <v>113</v>
       </c>
       <c r="F18" t="n">
-        <v>309091</v>
+        <v>165</v>
       </c>
       <c r="G18" t="n">
-        <v>-86.98</v>
+        <v>-95.8</v>
       </c>
       <c r="H18" t="n">
-        <v>-6.53</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>2001</v>
-      </c>
-      <c r="B19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" t="s">
-        <v>28</v>
-      </c>
-      <c r="D19" t="n">
-        <v>59914</v>
-      </c>
-      <c r="E19" t="n">
-        <v>147587</v>
-      </c>
-      <c r="F19" t="n">
-        <v>210485</v>
-      </c>
-      <c r="G19" t="n">
-        <v>-52.81</v>
-      </c>
-      <c r="H19" t="n">
-        <v>2.89</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>2007</v>
-      </c>
-      <c r="B20" t="s">
-        <v>8</v>
-      </c>
-      <c r="C20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" t="n">
-        <v>93991</v>
-      </c>
-      <c r="E20" t="n">
-        <v>114317</v>
-      </c>
-      <c r="F20" t="n">
-        <v>140404</v>
-      </c>
-      <c r="G20" t="n">
-        <v>-54.6</v>
-      </c>
-      <c r="H20" t="n">
-        <v>-13.35</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>1993</v>
-      </c>
-      <c r="B21" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" t="n">
-        <v>339406</v>
-      </c>
-      <c r="E21" t="n">
-        <v>1032599</v>
-      </c>
-      <c r="F21" t="n">
-        <v>1705841</v>
-      </c>
-      <c r="G21" t="n">
-        <v>-93.99</v>
-      </c>
-      <c r="H21" t="n">
-        <v>8.75</v>
+        <v>149.66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>